<commit_message>
aact-902: proj_tag_moc: Name the excel sheet of tagged terms ’Analysis Data’
</commit_message>
<xml_diff>
--- a/public/attachments/proj_tag_moc_terms.xlsx
+++ b/public/attachments/proj_tag_moc_terms.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tibbs001/work/aact-proj-1/public/attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B301B864-54A2-984D-9511-2FE591CDE20B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA0BE99-C784-AC4F-B74B-DA09C87EDF9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1120" windowWidth="24800" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="620" windowWidth="24800" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Analysis Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407"/>
   <extLst>

</xml_diff>